<commit_message>
[DG22-2616] adjust test description and rename constant variable URL path and Sheet name
</commit_message>
<xml_diff>
--- a/cypress/fixtures/data.xlsx
+++ b/cypress/fixtures/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felix/kororo/repository/dcceew-safeguard-rules-interface/cypress/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21F583CD-84A9-B04F-88C8-5BDF860C67BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31E145D9-6CC7-9941-B43B-B5E565B35D3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -764,7 +764,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>